<commit_message>
Nouveau projet avec début CRUD session+user+roles
</commit_message>
<xml_diff>
--- a/Docs/Répartition des tâches.xlsx
+++ b/Docs/Répartition des tâches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benoit\Documents\GitHub\Projet_planning_poker\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F306C5-BC7D-4F15-B812-6E585EA0FA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB5A0C3-57C7-49FA-B3FA-DAA5FDC8DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2304322C-D999-46F5-8333-EC45C352ADBC}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16212" windowHeight="9552" xr2:uid="{2304322C-D999-46F5-8333-EC45C352ADBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Benoit Danglades</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Front</t>
+  </si>
+  <si>
+    <t>Back</t>
   </si>
   <si>
     <t>BDD+Back</t>
@@ -453,7 +456,7 @@
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>